<commit_message>
system and device id that corresponds to NEST wiki added to solace metadata
</commit_message>
<xml_diff>
--- a/SolAce/solace_metadata.xlsx
+++ b/SolAce/solace_metadata.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wolfram\workspace\opendata_NEST\SolAce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{781D3D2F-89D4-46C1-895C-9431DD07CD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36603DA-C76D-4478-94CA-E8F4B088D380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="82365" yWindow="1965" windowWidth="21600" windowHeight="12660"/>
+    <workbookView xWindow="78420" yWindow="120" windowWidth="21600" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="solace_metadata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
   <si>
     <t>NumericID</t>
   </si>
@@ -191,12 +202,81 @@
   </si>
   <si>
     <t>Presence detection in the linving room [0/1]</t>
+  </si>
+  <si>
+    <t>System_Id</t>
+  </si>
+  <si>
+    <t>Device_Id</t>
+  </si>
+  <si>
+    <t>MET51</t>
+  </si>
+  <si>
+    <t>B870</t>
+  </si>
+  <si>
+    <t>U25M2</t>
+  </si>
+  <si>
+    <t>Y700</t>
+  </si>
+  <si>
+    <t>Y701</t>
+  </si>
+  <si>
+    <t>U25F1</t>
+  </si>
+  <si>
+    <t>M200</t>
+  </si>
+  <si>
+    <t>U25F2</t>
+  </si>
+  <si>
+    <t>U25F3</t>
+  </si>
+  <si>
+    <t>U25F4</t>
+  </si>
+  <si>
+    <t>B810</t>
+  </si>
+  <si>
+    <t>B811</t>
+  </si>
+  <si>
+    <t>U25M1</t>
+  </si>
+  <si>
+    <t>P890</t>
+  </si>
+  <si>
+    <t>U25N1</t>
+  </si>
+  <si>
+    <t>U25E3</t>
+  </si>
+  <si>
+    <t>T100</t>
+  </si>
+  <si>
+    <t>U25E1</t>
+  </si>
+  <si>
+    <t>P001</t>
+  </si>
+  <si>
+    <t>U25R2</t>
+  </si>
+  <si>
+    <t>U25R1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1030,11 +1110,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1046,7 +1126,7 @@
     <col min="5" max="5" width="19.765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1062,8 +1142,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>3200000</v>
       </c>
@@ -1079,8 +1165,14 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>3200008</v>
       </c>
@@ -1096,8 +1188,14 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>42180043</v>
       </c>
@@ -1113,8 +1211,14 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>42180045</v>
       </c>
@@ -1130,8 +1234,14 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>42180159</v>
       </c>
@@ -1147,8 +1257,14 @@
       <c r="E6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>42180160</v>
       </c>
@@ -1164,8 +1280,14 @@
       <c r="E7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>42180170</v>
       </c>
@@ -1181,8 +1303,14 @@
       <c r="E8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>42180171</v>
       </c>
@@ -1198,8 +1326,14 @@
       <c r="E9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>42180179</v>
       </c>
@@ -1215,8 +1349,14 @@
       <c r="E10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>42180187</v>
       </c>
@@ -1232,8 +1372,14 @@
       <c r="E11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>42180023</v>
       </c>
@@ -1249,8 +1395,14 @@
       <c r="E12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>42180034</v>
       </c>
@@ -1266,8 +1418,14 @@
       <c r="E13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>42180024</v>
       </c>
@@ -1283,8 +1441,14 @@
       <c r="E14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>42180035</v>
       </c>
@@ -1300,8 +1464,14 @@
       <c r="E15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>42160122</v>
       </c>
@@ -1317,8 +1487,14 @@
       <c r="E16" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>42160203</v>
       </c>
@@ -1334,8 +1510,14 @@
       <c r="E17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>42160278</v>
       </c>
@@ -1351,8 +1533,14 @@
       <c r="E18" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>42160255</v>
       </c>
@@ -1368,8 +1556,14 @@
       <c r="E19" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F19" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>42180007</v>
       </c>
@@ -1385,8 +1579,14 @@
       <c r="E20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>42180000</v>
       </c>
@@ -1401,6 +1601,12 @@
       </c>
       <c r="E21" t="s">
         <v>54</v>
+      </c>
+      <c r="F21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>